<commit_message>
Ran Evaluation with baseline model configuration
</commit_message>
<xml_diff>
--- a/RAGAS Questions.xlsx
+++ b/RAGAS Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MEng Project\MEng_Project_RAG_for_Defence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{495FAA8C-200E-4E34-A682-003519921EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6240CC4-7AC6-4622-9861-9822A5F76A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E34568A9-0812-4732-A47E-B037F315B3F5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E34568A9-0812-4732-A47E-B037F315B3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1900,10 +1900,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2223,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6867C8-B744-4899-AA30-E2808A8580BB}">
-  <dimension ref="A2:C102"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,23 +2232,34 @@
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -2260,10 +2267,10 @@
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -2271,32 +2278,32 @@
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -2304,10 +2311,10 @@
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -2315,10 +2322,10 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -2326,10 +2333,10 @@
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -2337,32 +2344,32 @@
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -2370,10 +2377,10 @@
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -2381,10 +2388,10 @@
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -2392,32 +2399,32 @@
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -2425,10 +2432,10 @@
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -2436,10 +2443,10 @@
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -2447,32 +2454,32 @@
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
         <v>65</v>
@@ -2480,10 +2487,10 @@
     </row>
     <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
         <v>65</v>
@@ -2491,21 +2498,21 @@
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>65</v>
@@ -2513,10 +2520,10 @@
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
         <v>65</v>
@@ -2524,10 +2531,10 @@
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>65</v>
@@ -2535,10 +2542,10 @@
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
         <v>65</v>
@@ -2546,10 +2553,10 @@
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>65</v>
@@ -2557,43 +2564,43 @@
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
         <v>85</v>
@@ -2601,10 +2608,10 @@
     </row>
     <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
         <v>85</v>
@@ -2612,21 +2619,21 @@
     </row>
     <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
         <v>85</v>
@@ -2634,10 +2641,10 @@
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
         <v>85</v>
@@ -2645,10 +2652,10 @@
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
         <v>85</v>
@@ -2656,10 +2663,10 @@
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
         <v>85</v>
@@ -2667,54 +2674,54 @@
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C44" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
         <v>107</v>
@@ -2722,10 +2729,10 @@
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
         <v>107</v>
@@ -2733,10 +2740,10 @@
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
         <v>107</v>
@@ -2744,10 +2751,10 @@
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
         <v>107</v>
@@ -2755,21 +2762,21 @@
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C49" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C50" t="s">
         <v>107</v>
@@ -2777,10 +2784,10 @@
     </row>
     <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C51" t="s">
         <v>107</v>
@@ -2788,21 +2795,21 @@
     </row>
     <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="C53" t="s">
         <v>128</v>
@@ -2810,21 +2817,21 @@
     </row>
     <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C54" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C55" t="s">
         <v>128</v>
@@ -2832,10 +2839,10 @@
     </row>
     <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C56" t="s">
         <v>128</v>
@@ -2843,10 +2850,10 @@
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C57" t="s">
         <v>128</v>
@@ -2854,10 +2861,10 @@
     </row>
     <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
         <v>128</v>
@@ -2865,10 +2872,10 @@
     </row>
     <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C59" t="s">
         <v>128</v>
@@ -2876,10 +2883,10 @@
     </row>
     <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C60" t="s">
         <v>128</v>
@@ -2887,32 +2894,32 @@
     </row>
     <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C62" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C63" t="s">
         <v>149</v>
@@ -2920,10 +2927,10 @@
     </row>
     <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C64" t="s">
         <v>149</v>
@@ -2931,10 +2938,10 @@
     </row>
     <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C65" t="s">
         <v>149</v>
@@ -2942,10 +2949,10 @@
     </row>
     <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C66" t="s">
         <v>149</v>
@@ -2953,10 +2960,10 @@
     </row>
     <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C67" t="s">
         <v>149</v>
@@ -2964,10 +2971,10 @@
     </row>
     <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C68" t="s">
         <v>149</v>
@@ -2975,10 +2982,10 @@
     </row>
     <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C69" t="s">
         <v>149</v>
@@ -2986,10 +2993,10 @@
     </row>
     <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C70" t="s">
         <v>149</v>
@@ -2997,32 +3004,32 @@
     </row>
     <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C71" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C73" t="s">
         <v>170</v>
@@ -3030,10 +3037,10 @@
     </row>
     <row r="74" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C74" t="s">
         <v>170</v>
@@ -3041,32 +3048,32 @@
     </row>
     <row r="75" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C75" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C76" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C77" t="s">
         <v>170</v>
@@ -3074,10 +3081,10 @@
     </row>
     <row r="78" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C78" t="s">
         <v>170</v>
@@ -3085,10 +3092,10 @@
     </row>
     <row r="79" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C79" t="s">
         <v>170</v>
@@ -3096,10 +3103,10 @@
     </row>
     <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C80" t="s">
         <v>170</v>
@@ -3107,10 +3114,10 @@
     </row>
     <row r="81" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C81" t="s">
         <v>170</v>
@@ -3118,32 +3125,32 @@
     </row>
     <row r="82" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C82" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C83" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C84" t="s">
         <v>191</v>
@@ -3151,10 +3158,10 @@
     </row>
     <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C85" t="s">
         <v>191</v>
@@ -3162,10 +3169,10 @@
     </row>
     <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C86" t="s">
         <v>191</v>
@@ -3173,10 +3180,10 @@
     </row>
     <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C87" t="s">
         <v>191</v>
@@ -3184,32 +3191,32 @@
     </row>
     <row r="88" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C88" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C89" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C90" t="s">
         <v>191</v>
@@ -3217,32 +3224,32 @@
     </row>
     <row r="91" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C91" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C92" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C93" t="s">
         <v>212</v>
@@ -3250,10 +3257,10 @@
     </row>
     <row r="94" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C94" t="s">
         <v>212</v>
@@ -3261,21 +3268,21 @@
     </row>
     <row r="95" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C95" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C96" t="s">
         <v>212</v>
@@ -3283,43 +3290,43 @@
     </row>
     <row r="97" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C97" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="C98" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="C99" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C100" t="s">
         <v>212</v>
@@ -3327,23 +3334,12 @@
     </row>
     <row r="101" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C101" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C102" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3354,6 +3350,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a8bb0526-feae-4db6-bc6d-fde4e2aa0c50" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064A3487AA3E5E04C924CD05BB33845BE" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8a8ab9203fce2aa0855331776c006022">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="56d92af7-ff2e-4d10-b07a-8ae38e12e248" xmlns:ns4="a8bb0526-feae-4db6-bc6d-fde4e2aa0c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8613b227c188d20b4491194b58678199" ns3:_="" ns4:_="">
     <xsd:import namespace="56d92af7-ff2e-4d10-b07a-8ae38e12e248"/>
@@ -3586,14 +3590,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a8bb0526-feae-4db6-bc6d-fde4e2aa0c50" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3604,6 +3600,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741BBC2C-96B4-47A3-BF7B-120063540924}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a8bb0526-feae-4db6-bc6d-fde4e2aa0c50"/>
+    <ds:schemaRef ds:uri="56d92af7-ff2e-4d10-b07a-8ae38e12e248"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79C62951-7B74-46E8-8E14-6A347DB0C4EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3622,23 +3635,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741BBC2C-96B4-47A3-BF7B-120063540924}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a8bb0526-feae-4db6-bc6d-fde4e2aa0c50"/>
-    <ds:schemaRef ds:uri="56d92af7-ff2e-4d10-b07a-8ae38e12e248"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6028E862-816B-4939-A77F-4ABBB7A27FB3}">
   <ds:schemaRefs>

</xml_diff>